<commit_message>
CHANGE THE PRIORITY ORDER ACCORDING TO QUES
</commit_message>
<xml_diff>
--- a/Comprehensive_Reaction_Analysis.xlsx
+++ b/Comprehensive_Reaction_Analysis.xlsx
@@ -565,7 +565,7 @@
         <v>1</v>
       </c>
       <c r="P2" t="n">
-        <v>3.75</v>
+        <v>4.4</v>
       </c>
     </row>
     <row r="3">
@@ -617,7 +617,7 @@
         <v>2</v>
       </c>
       <c r="P3" t="n">
-        <v>3.29380185933934</v>
+        <v>3.37155336908946</v>
       </c>
     </row>
     <row r="4">
@@ -669,7 +669,7 @@
         <v>3</v>
       </c>
       <c r="P4" t="n">
-        <v>1.13138454977107</v>
+        <v>0.6241629712659377</v>
       </c>
     </row>
     <row r="5">
@@ -721,7 +721,7 @@
         <v>1</v>
       </c>
       <c r="P5" t="n">
-        <v>3.75</v>
+        <v>4.4</v>
       </c>
     </row>
     <row r="6">
@@ -773,7 +773,7 @@
         <v>2</v>
       </c>
       <c r="P6" t="n">
-        <v>3.290451924886361</v>
+        <v>3.347926146658295</v>
       </c>
     </row>
     <row r="7">
@@ -825,7 +825,7 @@
         <v>3</v>
       </c>
       <c r="P7" t="n">
-        <v>1.131347705209858</v>
+        <v>0.6241340219678418</v>
       </c>
     </row>
     <row r="8">
@@ -877,7 +877,7 @@
         <v>1</v>
       </c>
       <c r="P8" t="n">
-        <v>3.75</v>
+        <v>4.4</v>
       </c>
     </row>
     <row r="9">
@@ -929,7 +929,7 @@
         <v>2</v>
       </c>
       <c r="P9" t="n">
-        <v>3.300645802549675</v>
+        <v>3.336389906470643</v>
       </c>
     </row>
     <row r="10">
@@ -981,7 +981,7 @@
         <v>3</v>
       </c>
       <c r="P10" t="n">
-        <v>1.131274370339598</v>
+        <v>0.6240764017126385</v>
       </c>
     </row>
     <row r="11">
@@ -1033,7 +1033,7 @@
         <v>1</v>
       </c>
       <c r="P11" t="n">
-        <v>3.42154471544715</v>
+        <v>3.702032520325195</v>
       </c>
     </row>
     <row r="12">
@@ -1085,7 +1085,7 @@
         <v>2</v>
       </c>
       <c r="P12" t="n">
-        <v>3.020894218609199</v>
+        <v>2.758747493241533</v>
       </c>
     </row>
     <row r="13">
@@ -1137,7 +1137,7 @@
         <v>3</v>
       </c>
       <c r="P13" t="n">
-        <v>1.532765258265685</v>
+        <v>1.475247813654563</v>
       </c>
     </row>
     <row r="14">
@@ -1189,7 +1189,7 @@
         <v>1</v>
       </c>
       <c r="P14" t="n">
-        <v>3.434897959183683</v>
+        <v>3.730408163265326</v>
       </c>
     </row>
     <row r="15">
@@ -1241,7 +1241,7 @@
         <v>2</v>
       </c>
       <c r="P15" t="n">
-        <v>3.046031867060472</v>
+        <v>2.795013647031681</v>
       </c>
     </row>
     <row r="16">
@@ -1293,7 +1293,7 @@
         <v>3</v>
       </c>
       <c r="P16" t="n">
-        <v>1.53273379617102</v>
+        <v>1.475223093437327</v>
       </c>
     </row>
     <row r="17">
@@ -1345,7 +1345,7 @@
         <v>1</v>
       </c>
       <c r="P17" t="n">
-        <v>3.458943089430901</v>
+        <v>3.781504065040667</v>
       </c>
     </row>
     <row r="18">
@@ -1397,7 +1397,7 @@
         <v>2</v>
       </c>
       <c r="P18" t="n">
-        <v>3.096011803769292</v>
+        <v>2.867116127102249</v>
       </c>
     </row>
     <row r="19">
@@ -1449,7 +1449,7 @@
         <v>3</v>
       </c>
       <c r="P19" t="n">
-        <v>1.532686590664138</v>
+        <v>1.475186003396205</v>
       </c>
     </row>
     <row r="20">
@@ -1501,7 +1501,7 @@
         <v>1</v>
       </c>
       <c r="P20" t="n">
-        <v>3.514705882352941</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="21">
@@ -1553,7 +1553,7 @@
         <v>2</v>
       </c>
       <c r="P21" t="n">
-        <v>3.039270521387545</v>
+        <v>2.785151743897122</v>
       </c>
     </row>
     <row r="22">
@@ -1605,7 +1605,7 @@
         <v>3</v>
       </c>
       <c r="P22" t="n">
-        <v>1.532456073524198</v>
+        <v>1.475004882786253</v>
       </c>
     </row>
     <row r="23">
@@ -1657,7 +1657,7 @@
         <v>1</v>
       </c>
       <c r="P23" t="n">
-        <v>3.524509803921571</v>
+        <v>3.920833333333339</v>
       </c>
     </row>
     <row r="24">
@@ -1709,7 +1709,7 @@
         <v>2</v>
       </c>
       <c r="P24" t="n">
-        <v>3.066441004674914</v>
+        <v>2.824366798369596</v>
       </c>
     </row>
     <row r="25">
@@ -1761,7 +1761,7 @@
         <v>3</v>
       </c>
       <c r="P25" t="n">
-        <v>1.532439015562197</v>
+        <v>1.474991480101823</v>
       </c>
     </row>
     <row r="26">
@@ -1813,7 +1813,7 @@
         <v>1</v>
       </c>
       <c r="P26" t="n">
-        <v>3.538753056234706</v>
+        <v>3.951100244498751</v>
       </c>
     </row>
     <row r="27">
@@ -1865,7 +1865,7 @@
         <v>2</v>
       </c>
       <c r="P27" t="n">
-        <v>3.12008737336452</v>
+        <v>2.901803361749447</v>
       </c>
     </row>
     <row r="28">
@@ -1917,7 +1917,7 @@
         <v>3</v>
       </c>
       <c r="P28" t="n">
-        <v>1.532415467726173</v>
+        <v>1.474972978230662</v>
       </c>
     </row>
     <row r="29">
@@ -1969,7 +1969,7 @@
         <v>1</v>
       </c>
       <c r="P29" t="n">
-        <v>3.723333333333302</v>
+        <v>4.343333333333266</v>
       </c>
     </row>
     <row r="30">
@@ -2021,7 +2021,7 @@
         <v>2</v>
       </c>
       <c r="P30" t="n">
-        <v>2.968757051021184</v>
+        <v>2.683396196626719</v>
       </c>
     </row>
     <row r="31">
@@ -2073,7 +2073,7 @@
         <v>3</v>
       </c>
       <c r="P31" t="n">
-        <v>1.531962756819522</v>
+        <v>1.474617276804007</v>
       </c>
     </row>
     <row r="32">
@@ -2125,7 +2125,7 @@
         <v>1</v>
       </c>
       <c r="P32" t="n">
-        <v>3.716666666666698</v>
+        <v>4.329166666666734</v>
       </c>
     </row>
     <row r="33">
@@ -2177,7 +2177,7 @@
         <v>2</v>
       </c>
       <c r="P33" t="n">
-        <v>2.99086996767215</v>
+        <v>2.715338346136939</v>
       </c>
     </row>
     <row r="34">
@@ -2229,7 +2229,7 @@
         <v>3</v>
       </c>
       <c r="P34" t="n">
-        <v>1.531966160090648</v>
+        <v>1.474619950802749</v>
       </c>
     </row>
     <row r="35">
@@ -2281,7 +2281,7 @@
         <v>1</v>
       </c>
       <c r="P35" t="n">
-        <v>3.720000000000047</v>
+        <v>4.336250000000101</v>
       </c>
     </row>
     <row r="36">
@@ -2333,7 +2333,7 @@
         <v>2</v>
       </c>
       <c r="P36" t="n">
-        <v>3.034480386352751</v>
+        <v>2.778322100352302</v>
       </c>
     </row>
     <row r="37">
@@ -2385,7 +2385,7 @@
         <v>3</v>
       </c>
       <c r="P37" t="n">
-        <v>1.531964458445159</v>
+        <v>1.474618613795579</v>
       </c>
     </row>
     <row r="38">
@@ -2437,7 +2437,7 @@
         <v>1</v>
       </c>
       <c r="P38" t="n">
-        <v>3.75</v>
+        <v>4.4</v>
       </c>
     </row>
     <row r="39">
@@ -2489,7 +2489,7 @@
         <v>2</v>
       </c>
       <c r="P39" t="n">
-        <v>2.852106931340572</v>
+        <v>2.51506446418664</v>
       </c>
     </row>
     <row r="40">
@@ -2541,7 +2541,7 @@
         <v>3</v>
       </c>
       <c r="P40" t="n">
-        <v>1.531915120720758</v>
+        <v>1.474579848440692</v>
       </c>
     </row>
     <row r="41">
@@ -2593,7 +2593,7 @@
         <v>1</v>
       </c>
       <c r="P41" t="n">
-        <v>3.75</v>
+        <v>4.4</v>
       </c>
     </row>
     <row r="42">
@@ -2645,7 +2645,7 @@
         <v>2</v>
       </c>
       <c r="P42" t="n">
-        <v>2.86670542959775</v>
+        <v>2.536153784244761</v>
       </c>
     </row>
     <row r="43">
@@ -2697,7 +2697,7 @@
         <v>3</v>
       </c>
       <c r="P43" t="n">
-        <v>1.531914440186753</v>
+        <v>1.474579313735402</v>
       </c>
     </row>
     <row r="44">
@@ -2749,7 +2749,7 @@
         <v>1</v>
       </c>
       <c r="P44" t="n">
-        <v>3.75</v>
+        <v>4.4</v>
       </c>
     </row>
     <row r="45">
@@ -2801,7 +2801,7 @@
         <v>2</v>
       </c>
       <c r="P45" t="n">
-        <v>2.895587298443142</v>
+        <v>2.577869897105686</v>
       </c>
     </row>
     <row r="46">
@@ -2853,7 +2853,7 @@
         <v>3</v>
       </c>
       <c r="P46" t="n">
-        <v>1.531914780454039</v>
+        <v>1.47457958108827</v>
       </c>
     </row>
   </sheetData>
@@ -2944,10 +2944,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3.636890300438067</v>
+        <v>4.159641888430892</v>
       </c>
       <c r="C2" t="n">
-        <v>0.8849485481704872</v>
+        <v>0.7835335425850183</v>
       </c>
       <c r="D2" t="n">
         <v>15</v>
@@ -2984,10 +2984,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3.058809562671257</v>
+        <v>2.852947558817539</v>
       </c>
       <c r="C3" t="n">
-        <v>0.8771686563038753</v>
+        <v>0.7860433831129233</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
@@ -3024,10 +3024,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1.452076036263388</v>
+        <v>1.30470628208133</v>
       </c>
       <c r="C4" t="n">
-        <v>0.8617936859177725</v>
+        <v>0.746106633459375</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>

</xml_diff>